<commit_message>
Major changes for finalisation of the project :)
</commit_message>
<xml_diff>
--- a/ai/nn/grid_search.xlsx
+++ b/ai/nn/grid_search.xlsx
@@ -482,10 +482,10 @@
         <v>40</v>
       </c>
       <c r="F2" t="n">
-        <v>-4.860656747125383e-07</v>
+        <v>-1.796112343456927e-06</v>
       </c>
       <c r="G2" t="n">
-        <v>2.519894706324488e-07</v>
+        <v>1.76695036201989e-06</v>
       </c>
     </row>
     <row r="3">
@@ -505,10 +505,10 @@
         <v>50</v>
       </c>
       <c r="F3" t="n">
-        <v>-2.576211592268107e-07</v>
+        <v>-7.517602814076269e-07</v>
       </c>
       <c r="G3" t="n">
-        <v>9.201883775359337e-08</v>
+        <v>5.863039089722849e-07</v>
       </c>
     </row>
     <row r="4">
@@ -528,10 +528,10 @@
         <v>60</v>
       </c>
       <c r="F4" t="n">
-        <v>-7.292791499170344e-07</v>
+        <v>-2.123031681192402e-06</v>
       </c>
       <c r="G4" t="n">
-        <v>4.409393421895771e-07</v>
+        <v>1.487409864198573e-06</v>
       </c>
     </row>
     <row r="5">
@@ -551,10 +551,10 @@
         <v>40</v>
       </c>
       <c r="F5" t="n">
-        <v>-3.904909837774123e-07</v>
+        <v>-5.905237966067131e-07</v>
       </c>
       <c r="G5" t="n">
-        <v>2.173574494468948e-07</v>
+        <v>6.857122142964479e-08</v>
       </c>
     </row>
     <row r="6">
@@ -574,10 +574,10 @@
         <v>50</v>
       </c>
       <c r="F6" t="n">
-        <v>-3.878962080454767e-07</v>
+        <v>-2.14866396433835e-06</v>
       </c>
       <c r="G6" t="n">
-        <v>3.386149069943137e-07</v>
+        <v>2.497080239898564e-06</v>
       </c>
     </row>
     <row r="7">
@@ -597,10 +597,10 @@
         <v>60</v>
       </c>
       <c r="F7" t="n">
-        <v>-5.474953111566651e-07</v>
+        <v>-4.646138596239986e-07</v>
       </c>
       <c r="G7" t="n">
-        <v>3.292702169661305e-07</v>
+        <v>2.619487597240604e-07</v>
       </c>
     </row>
     <row r="8">
@@ -620,10 +620,10 @@
         <v>40</v>
       </c>
       <c r="F8" t="n">
-        <v>-7.309798380590058e-07</v>
+        <v>-8.905572786081425e-07</v>
       </c>
       <c r="G8" t="n">
-        <v>3.600798193326294e-07</v>
+        <v>5.215298321440924e-07</v>
       </c>
     </row>
     <row r="9">
@@ -643,10 +643,10 @@
         <v>50</v>
       </c>
       <c r="F9" t="n">
-        <v>-8.393373472263013e-07</v>
+        <v>-1.204182721127126e-06</v>
       </c>
       <c r="G9" t="n">
-        <v>7.230333980468741e-07</v>
+        <v>5.649459388657275e-07</v>
       </c>
     </row>
     <row r="10">
@@ -666,10 +666,10 @@
         <v>60</v>
       </c>
       <c r="F10" t="n">
-        <v>-7.760016903437719e-07</v>
+        <v>-1.264607703403029e-06</v>
       </c>
       <c r="G10" t="n">
-        <v>5.086176986240951e-07</v>
+        <v>6.505861088058283e-07</v>
       </c>
     </row>
     <row r="11">
@@ -689,10 +689,10 @@
         <v>40</v>
       </c>
       <c r="F11" t="n">
-        <v>-1.911169583239854e-07</v>
+        <v>-2.68831453023207e-07</v>
       </c>
       <c r="G11" t="n">
-        <v>1.009678697296845e-07</v>
+        <v>3.719343344895759e-08</v>
       </c>
     </row>
     <row r="12">
@@ -712,10 +712,10 @@
         <v>50</v>
       </c>
       <c r="F12" t="n">
-        <v>-1.578406297787771e-07</v>
+        <v>-1.279534109928149e-06</v>
       </c>
       <c r="G12" t="n">
-        <v>1.042133447398737e-07</v>
+        <v>1.468297842498958e-06</v>
       </c>
     </row>
     <row r="13">
@@ -735,10 +735,10 @@
         <v>60</v>
       </c>
       <c r="F13" t="n">
-        <v>-7.549761468311438e-07</v>
+        <v>-3.337392880152269e-07</v>
       </c>
       <c r="G13" t="n">
-        <v>4.936959109148284e-07</v>
+        <v>2.682989176872714e-07</v>
       </c>
     </row>
     <row r="14">
@@ -758,10 +758,10 @@
         <v>40</v>
       </c>
       <c r="F14" t="n">
-        <v>-5.796123598270242e-07</v>
+        <v>-3.325297582992903e-07</v>
       </c>
       <c r="G14" t="n">
-        <v>3.151132271143615e-07</v>
+        <v>2.017866986051158e-07</v>
       </c>
     </row>
     <row r="15">
@@ -781,10 +781,10 @@
         <v>50</v>
       </c>
       <c r="F15" t="n">
-        <v>-9.825145596896927e-07</v>
+        <v>-3.025493556027669e-07</v>
       </c>
       <c r="G15" t="n">
-        <v>9.301833685114273e-07</v>
+        <v>1.921681547154633e-07</v>
       </c>
     </row>
     <row r="16">
@@ -804,10 +804,10 @@
         <v>60</v>
       </c>
       <c r="F16" t="n">
-        <v>-1.459387595230109e-06</v>
+        <v>-2.363969993442045e-07</v>
       </c>
       <c r="G16" t="n">
-        <v>8.232227524978807e-07</v>
+        <v>8.772763351332577e-08</v>
       </c>
     </row>
     <row r="17">
@@ -827,10 +827,10 @@
         <v>40</v>
       </c>
       <c r="F17" t="n">
-        <v>-3.437018775270592e-07</v>
+        <v>-2.78744033749708e-07</v>
       </c>
       <c r="G17" t="n">
-        <v>8.877017000757663e-08</v>
+        <v>1.172460171609518e-07</v>
       </c>
     </row>
     <row r="18">
@@ -850,10 +850,10 @@
         <v>50</v>
       </c>
       <c r="F18" t="n">
-        <v>-1.461626394337172e-06</v>
+        <v>-3.091165713908883e-07</v>
       </c>
       <c r="G18" t="n">
-        <v>1.075648120319738e-06</v>
+        <v>1.45845972001509e-07</v>
       </c>
     </row>
     <row r="19">
@@ -873,10 +873,10 @@
         <v>60</v>
       </c>
       <c r="F19" t="n">
-        <v>-1.150178807524444e-06</v>
+        <v>-1.538551995258939e-07</v>
       </c>
       <c r="G19" t="n">
-        <v>9.848074430081869e-07</v>
+        <v>6.647228680767493e-08</v>
       </c>
     </row>
     <row r="20">
@@ -896,10 +896,10 @@
         <v>40</v>
       </c>
       <c r="F20" t="n">
-        <v>-1.443015482070273e-07</v>
+        <v>-9.001069813367465e-08</v>
       </c>
       <c r="G20" t="n">
-        <v>2.672299023111312e-08</v>
+        <v>2.066700976073247e-09</v>
       </c>
     </row>
     <row r="21">
@@ -919,10 +919,10 @@
         <v>50</v>
       </c>
       <c r="F21" t="n">
-        <v>-1.290406584188531e-07</v>
+        <v>-1.375117724023561e-07</v>
       </c>
       <c r="G21" t="n">
-        <v>6.909570868262442e-08</v>
+        <v>3.180081994104382e-08</v>
       </c>
     </row>
     <row r="22">
@@ -942,10 +942,10 @@
         <v>60</v>
       </c>
       <c r="F22" t="n">
-        <v>-1.04868958637303e-07</v>
+        <v>-1.469330069598687e-07</v>
       </c>
       <c r="G22" t="n">
-        <v>4.966524857660693e-08</v>
+        <v>1.28216206181269e-08</v>
       </c>
     </row>
     <row r="23">
@@ -965,10 +965,10 @@
         <v>40</v>
       </c>
       <c r="F23" t="n">
-        <v>-4.100184788328321e-07</v>
+        <v>-1.805930351589824e-07</v>
       </c>
       <c r="G23" t="n">
-        <v>3.192793720467097e-07</v>
+        <v>9.948076320833375e-08</v>
       </c>
     </row>
     <row r="24">
@@ -988,10 +988,10 @@
         <v>50</v>
       </c>
       <c r="F24" t="n">
-        <v>-4.436441023706434e-07</v>
+        <v>-2.270969738131832e-07</v>
       </c>
       <c r="G24" t="n">
-        <v>2.582382925699896e-07</v>
+        <v>1.090799154161676e-07</v>
       </c>
     </row>
     <row r="25">
@@ -1011,10 +1011,10 @@
         <v>60</v>
       </c>
       <c r="F25" t="n">
-        <v>-3.465234236329847e-07</v>
+        <v>-1.048424712680054e-07</v>
       </c>
       <c r="G25" t="n">
-        <v>9.351193776987157e-08</v>
+        <v>1.859721927828094e-08</v>
       </c>
     </row>
     <row r="26">
@@ -1034,10 +1034,10 @@
         <v>40</v>
       </c>
       <c r="F26" t="n">
-        <v>-8.049041923746865e-07</v>
+        <v>-2.240635195781667e-07</v>
       </c>
       <c r="G26" t="n">
-        <v>3.668959601802331e-07</v>
+        <v>6.572690844984389e-08</v>
       </c>
     </row>
     <row r="27">
@@ -1057,10 +1057,10 @@
         <v>50</v>
       </c>
       <c r="F27" t="n">
-        <v>-1.934558991764462e-06</v>
+        <v>-8.361311655360081e-08</v>
       </c>
       <c r="G27" t="n">
-        <v>2.475344628922028e-06</v>
+        <v>1.373352678530306e-08</v>
       </c>
     </row>
     <row r="28">
@@ -1080,10 +1080,10 @@
         <v>60</v>
       </c>
       <c r="F28" t="n">
-        <v>-2.864385157045922e-06</v>
+        <v>-1.209754894956545e-07</v>
       </c>
       <c r="G28" t="n">
-        <v>1.341967548111334e-06</v>
+        <v>3.664203325361719e-08</v>
       </c>
     </row>
     <row r="29">
@@ -1103,10 +1103,10 @@
         <v>40</v>
       </c>
       <c r="F29" t="n">
-        <v>-6.718500505610346e-07</v>
+        <v>-8.863374740496041e-07</v>
       </c>
       <c r="G29" t="n">
-        <v>2.12357188511526e-07</v>
+        <v>2.290724390916624e-07</v>
       </c>
     </row>
     <row r="30">
@@ -1126,10 +1126,10 @@
         <v>50</v>
       </c>
       <c r="F30" t="n">
-        <v>-5.952073517440633e-07</v>
+        <v>-9.200680442549384e-07</v>
       </c>
       <c r="G30" t="n">
-        <v>3.081040374855338e-07</v>
+        <v>4.92148822007401e-07</v>
       </c>
     </row>
     <row r="31">
@@ -1149,10 +1149,10 @@
         <v>60</v>
       </c>
       <c r="F31" t="n">
-        <v>-5.651529140738112e-07</v>
+        <v>-5.694290458816605e-06</v>
       </c>
       <c r="G31" t="n">
-        <v>3.074919193830717e-07</v>
+        <v>6.370098824321722e-06</v>
       </c>
     </row>
     <row r="32">
@@ -1172,10 +1172,10 @@
         <v>40</v>
       </c>
       <c r="F32" t="n">
-        <v>-3.014883475799916e-07</v>
+        <v>-9.60764492969903e-07</v>
       </c>
       <c r="G32" t="n">
-        <v>1.381288635628212e-07</v>
+        <v>4.278238009988725e-07</v>
       </c>
     </row>
     <row r="33">
@@ -1195,10 +1195,10 @@
         <v>50</v>
       </c>
       <c r="F33" t="n">
-        <v>-2.611724048556133e-07</v>
+        <v>-1.576824023369298e-06</v>
       </c>
       <c r="G33" t="n">
-        <v>9.320543327817847e-08</v>
+        <v>4.60297061134682e-07</v>
       </c>
     </row>
     <row r="34">
@@ -1218,10 +1218,10 @@
         <v>60</v>
       </c>
       <c r="F34" t="n">
-        <v>-1.683367365135484e-06</v>
+        <v>-5.09966765937278e-07</v>
       </c>
       <c r="G34" t="n">
-        <v>1.99795002364697e-06</v>
+        <v>2.159043566022506e-07</v>
       </c>
     </row>
     <row r="35">
@@ -1241,10 +1241,10 @@
         <v>40</v>
       </c>
       <c r="F35" t="n">
-        <v>-4.354811438791982e-07</v>
+        <v>-1.114359280575335e-06</v>
       </c>
       <c r="G35" t="n">
-        <v>2.426330588175284e-07</v>
+        <v>5.348122289175433e-07</v>
       </c>
     </row>
     <row r="36">
@@ -1264,10 +1264,10 @@
         <v>50</v>
       </c>
       <c r="F36" t="n">
-        <v>-3.679717072613229e-07</v>
+        <v>-4.5556110952001e-07</v>
       </c>
       <c r="G36" t="n">
-        <v>2.774584885255259e-07</v>
+        <v>1.500399964080035e-07</v>
       </c>
     </row>
     <row r="37">
@@ -1287,10 +1287,10 @@
         <v>60</v>
       </c>
       <c r="F37" t="n">
-        <v>-3.726265161606401e-06</v>
+        <v>-2.136296129146203e-06</v>
       </c>
       <c r="G37" t="n">
-        <v>4.127103712040324e-06</v>
+        <v>1.1797896756368e-06</v>
       </c>
     </row>
     <row r="38">
@@ -1310,10 +1310,10 @@
         <v>40</v>
       </c>
       <c r="F38" t="n">
-        <v>-3.836623193690747e-07</v>
+        <v>-1.062248576449358e-06</v>
       </c>
       <c r="G38" t="n">
-        <v>1.979748312730074e-07</v>
+        <v>3.545626360010267e-07</v>
       </c>
     </row>
     <row r="39">
@@ -1333,10 +1333,10 @@
         <v>50</v>
       </c>
       <c r="F39" t="n">
-        <v>-3.782614600282411e-07</v>
+        <v>-4.973520676094663e-07</v>
       </c>
       <c r="G39" t="n">
-        <v>1.890989342674496e-07</v>
+        <v>1.6379319299946e-07</v>
       </c>
     </row>
     <row r="40">
@@ -1356,10 +1356,10 @@
         <v>60</v>
       </c>
       <c r="F40" t="n">
-        <v>-1.708347284413143e-07</v>
+        <v>-2.516259749129009e-06</v>
       </c>
       <c r="G40" t="n">
-        <v>7.400870366718466e-08</v>
+        <v>2.935825343178932e-06</v>
       </c>
     </row>
     <row r="41">
@@ -1379,10 +1379,10 @@
         <v>40</v>
       </c>
       <c r="F41" t="n">
-        <v>-5.062363706561894e-07</v>
+        <v>-6.746510790106659e-07</v>
       </c>
       <c r="G41" t="n">
-        <v>4.297361334462472e-07</v>
+        <v>4.151605227996006e-07</v>
       </c>
     </row>
     <row r="42">
@@ -1402,10 +1402,10 @@
         <v>50</v>
       </c>
       <c r="F42" t="n">
-        <v>-3.562850924095542e-07</v>
+        <v>-6.933892681341671e-07</v>
       </c>
       <c r="G42" t="n">
-        <v>7.567795364022832e-08</v>
+        <v>3.391655512397763e-07</v>
       </c>
     </row>
     <row r="43">
@@ -1425,10 +1425,10 @@
         <v>60</v>
       </c>
       <c r="F43" t="n">
-        <v>-8.159183388262053e-07</v>
+        <v>-1.861974265136242e-07</v>
       </c>
       <c r="G43" t="n">
-        <v>8.433988761817389e-07</v>
+        <v>2.189910542084246e-08</v>
       </c>
     </row>
     <row r="44">
@@ -1448,10 +1448,10 @@
         <v>40</v>
       </c>
       <c r="F44" t="n">
-        <v>-5.630122674719602e-07</v>
+        <v>-2.328555634012307e-07</v>
       </c>
       <c r="G44" t="n">
-        <v>3.566864242894586e-07</v>
+        <v>7.758944842102524e-08</v>
       </c>
     </row>
     <row r="45">
@@ -1471,10 +1471,10 @@
         <v>50</v>
       </c>
       <c r="F45" t="n">
-        <v>-4.188464335883785e-07</v>
+        <v>-1.783738206597607e-06</v>
       </c>
       <c r="G45" t="n">
-        <v>2.426995618427661e-07</v>
+        <v>1.14395015718935e-06</v>
       </c>
     </row>
     <row r="46">
@@ -1494,10 +1494,10 @@
         <v>60</v>
       </c>
       <c r="F46" t="n">
-        <v>-6.57750173702462e-07</v>
+        <v>-1.202304140897227e-06</v>
       </c>
       <c r="G46" t="n">
-        <v>4.008588548002783e-07</v>
+        <v>8.217729275747913e-07</v>
       </c>
     </row>
     <row r="47">
@@ -1517,10 +1517,10 @@
         <v>40</v>
       </c>
       <c r="F47" t="n">
-        <v>-4.146877289635083e-07</v>
+        <v>-1.815369415167182e-07</v>
       </c>
       <c r="G47" t="n">
-        <v>2.57734657312032e-07</v>
+        <v>5.430496460935613e-08</v>
       </c>
     </row>
     <row r="48">
@@ -1540,10 +1540,10 @@
         <v>50</v>
       </c>
       <c r="F48" t="n">
-        <v>-1.62470840416885e-07</v>
+        <v>-6.027747182615015e-07</v>
       </c>
       <c r="G48" t="n">
-        <v>5.544372845880141e-08</v>
+        <v>4.831994493654933e-07</v>
       </c>
     </row>
     <row r="49">
@@ -1563,10 +1563,10 @@
         <v>60</v>
       </c>
       <c r="F49" t="n">
-        <v>-2.113695477615394e-07</v>
+        <v>-1.405830894011287e-07</v>
       </c>
       <c r="G49" t="n">
-        <v>1.036690527075779e-07</v>
+        <v>7.260577678664343e-09</v>
       </c>
     </row>
     <row r="50">
@@ -1586,10 +1586,10 @@
         <v>40</v>
       </c>
       <c r="F50" t="n">
-        <v>-3.983309351455391e-07</v>
+        <v>-1.090292781413906e-07</v>
       </c>
       <c r="G50" t="n">
-        <v>3.222914675454627e-07</v>
+        <v>2.538531077459808e-08</v>
       </c>
     </row>
     <row r="51">
@@ -1609,10 +1609,10 @@
         <v>50</v>
       </c>
       <c r="F51" t="n">
-        <v>-1.016905226192868e-07</v>
+        <v>-1.067106457113347e-07</v>
       </c>
       <c r="G51" t="n">
-        <v>4.342940774926683e-08</v>
+        <v>1.114409377056923e-08</v>
       </c>
     </row>
     <row r="52">
@@ -1632,10 +1632,10 @@
         <v>60</v>
       </c>
       <c r="F52" t="n">
-        <v>-3.338095048211129e-07</v>
+        <v>-2.776031735564883e-07</v>
       </c>
       <c r="G52" t="n">
-        <v>2.45170537823392e-07</v>
+        <v>1.173143470317005e-07</v>
       </c>
     </row>
     <row r="53">
@@ -1655,10 +1655,10 @@
         <v>40</v>
       </c>
       <c r="F53" t="n">
-        <v>-3.557932737287695e-07</v>
+        <v>-8.500404610975811e-08</v>
       </c>
       <c r="G53" t="n">
-        <v>9.236190308934985e-08</v>
+        <v>2.710931310764748e-08</v>
       </c>
     </row>
     <row r="54">
@@ -1678,10 +1678,10 @@
         <v>50</v>
       </c>
       <c r="F54" t="n">
-        <v>-5.79049768218556e-07</v>
+        <v>-3.272980522239378e-07</v>
       </c>
       <c r="G54" t="n">
-        <v>3.862254644158852e-07</v>
+        <v>2.152789810626827e-07</v>
       </c>
     </row>
     <row r="55">
@@ -1701,10 +1701,10 @@
         <v>60</v>
       </c>
       <c r="F55" t="n">
-        <v>-5.388780279324761e-07</v>
+        <v>-1.189752223722602e-07</v>
       </c>
       <c r="G55" t="n">
-        <v>2.326340407625034e-07</v>
+        <v>3.17160922817471e-08</v>
       </c>
     </row>
     <row r="56">
@@ -1724,10 +1724,10 @@
         <v>40</v>
       </c>
       <c r="F56" t="n">
-        <v>-1.366322940003673e-06</v>
+        <v>-1.331582448324408e-06</v>
       </c>
       <c r="G56" t="n">
-        <v>3.787126084964988e-07</v>
+        <v>3.768399299677323e-07</v>
       </c>
     </row>
     <row r="57">
@@ -1747,10 +1747,10 @@
         <v>50</v>
       </c>
       <c r="F57" t="n">
-        <v>-7.060532991871209e-07</v>
+        <v>-3.346795970402759e-06</v>
       </c>
       <c r="G57" t="n">
-        <v>1.674884335931132e-07</v>
+        <v>8.568730864928782e-07</v>
       </c>
     </row>
     <row r="58">
@@ -1770,10 +1770,10 @@
         <v>60</v>
       </c>
       <c r="F58" t="n">
-        <v>-1.106674453335931e-06</v>
+        <v>-1.095635134018407e-06</v>
       </c>
       <c r="G58" t="n">
-        <v>7.327372058978907e-07</v>
+        <v>2.677018042787322e-07</v>
       </c>
     </row>
     <row r="59">
@@ -1793,10 +1793,10 @@
         <v>40</v>
       </c>
       <c r="F59" t="n">
-        <v>-6.614307705647106e-07</v>
+        <v>-9.440581983617456e-07</v>
       </c>
       <c r="G59" t="n">
-        <v>3.799642970870382e-07</v>
+        <v>9.965689764366469e-08</v>
       </c>
     </row>
     <row r="60">
@@ -1816,10 +1816,10 @@
         <v>50</v>
       </c>
       <c r="F60" t="n">
-        <v>-5.068568702928094e-07</v>
+        <v>-2.611759017842105e-06</v>
       </c>
       <c r="G60" t="n">
-        <v>2.565850520824067e-07</v>
+        <v>1.48852447363023e-06</v>
       </c>
     </row>
     <row r="61">
@@ -1839,10 +1839,10 @@
         <v>60</v>
       </c>
       <c r="F61" t="n">
-        <v>-8.424691983194804e-07</v>
+        <v>-7.501531892647101e-06</v>
       </c>
       <c r="G61" t="n">
-        <v>6.854647885289966e-07</v>
+        <v>6.77865921114918e-06</v>
       </c>
     </row>
     <row r="62">
@@ -1862,10 +1862,10 @@
         <v>40</v>
       </c>
       <c r="F62" t="n">
-        <v>-1.343004419356551e-06</v>
+        <v>-2.719550105201919e-06</v>
       </c>
       <c r="G62" t="n">
-        <v>6.936265748270889e-07</v>
+        <v>1.686412529592774e-06</v>
       </c>
     </row>
     <row r="63">
@@ -1885,10 +1885,10 @@
         <v>50</v>
       </c>
       <c r="F63" t="n">
-        <v>-7.209199040637138e-07</v>
+        <v>-2.120500643450274e-06</v>
       </c>
       <c r="G63" t="n">
-        <v>3.688725067247923e-07</v>
+        <v>4.870073090281995e-07</v>
       </c>
     </row>
     <row r="64">
@@ -1908,10 +1908,10 @@
         <v>60</v>
       </c>
       <c r="F64" t="n">
-        <v>-9.982060193168231e-07</v>
+        <v>-8.123566632203276e-07</v>
       </c>
       <c r="G64" t="n">
-        <v>2.19120123947098e-07</v>
+        <v>2.928905986189997e-07</v>
       </c>
     </row>
     <row r="65">
@@ -1931,10 +1931,10 @@
         <v>40</v>
       </c>
       <c r="F65" t="n">
-        <v>-5.579212289122149e-07</v>
+        <v>-5.281860362655796e-07</v>
       </c>
       <c r="G65" t="n">
-        <v>2.15993588545234e-07</v>
+        <v>2.112248835505304e-08</v>
       </c>
     </row>
     <row r="66">
@@ -1954,10 +1954,10 @@
         <v>50</v>
       </c>
       <c r="F66" t="n">
-        <v>-5.621538257543926e-07</v>
+        <v>-4.332069116572644e-06</v>
       </c>
       <c r="G66" t="n">
-        <v>3.158081476245467e-07</v>
+        <v>5.001508955191291e-06</v>
       </c>
     </row>
     <row r="67">
@@ -1977,10 +1977,10 @@
         <v>60</v>
       </c>
       <c r="F67" t="n">
-        <v>-3.823307315310307e-07</v>
+        <v>-9.007148371337648e-07</v>
       </c>
       <c r="G67" t="n">
-        <v>1.046750647788661e-07</v>
+        <v>3.7214107244611e-07</v>
       </c>
     </row>
     <row r="68">
@@ -2000,10 +2000,10 @@
         <v>40</v>
       </c>
       <c r="F68" t="n">
-        <v>-3.113407577264013e-06</v>
+        <v>-3.471143816181386e-07</v>
       </c>
       <c r="G68" t="n">
-        <v>2.711639124167124e-06</v>
+        <v>7.461521526941438e-08</v>
       </c>
     </row>
     <row r="69">
@@ -2023,10 +2023,10 @@
         <v>50</v>
       </c>
       <c r="F69" t="n">
-        <v>-2.091598558143086e-07</v>
+        <v>-9.674227444076104e-07</v>
       </c>
       <c r="G69" t="n">
-        <v>1.31028409212284e-07</v>
+        <v>5.891543667382416e-07</v>
       </c>
     </row>
     <row r="70">
@@ -2046,10 +2046,10 @@
         <v>60</v>
       </c>
       <c r="F70" t="n">
-        <v>-7.021627305811131e-07</v>
+        <v>-2.841690616716328e-07</v>
       </c>
       <c r="G70" t="n">
-        <v>7.613206551671091e-07</v>
+        <v>9.469562048533069e-08</v>
       </c>
     </row>
     <row r="71">
@@ -2069,10 +2069,10 @@
         <v>40</v>
       </c>
       <c r="F71" t="n">
-        <v>-5.219150195268628e-07</v>
+        <v>-6.552333663276142e-07</v>
       </c>
       <c r="G71" t="n">
-        <v>4.921056529219656e-07</v>
+        <v>3.474368725570029e-07</v>
       </c>
     </row>
     <row r="72">
@@ -2092,10 +2092,10 @@
         <v>50</v>
       </c>
       <c r="F72" t="n">
-        <v>-2.604140470862025e-07</v>
+        <v>-6.708954134498862e-07</v>
       </c>
       <c r="G72" t="n">
-        <v>1.699192426622123e-07</v>
+        <v>2.018343815679029e-07</v>
       </c>
     </row>
     <row r="73">
@@ -2115,10 +2115,10 @@
         <v>60</v>
       </c>
       <c r="F73" t="n">
-        <v>-2.687124992666027e-06</v>
+        <v>-4.366526276319812e-07</v>
       </c>
       <c r="G73" t="n">
-        <v>2.849679064671266e-06</v>
+        <v>1.928800537628643e-07</v>
       </c>
     </row>
     <row r="74">
@@ -2138,10 +2138,10 @@
         <v>40</v>
       </c>
       <c r="F74" t="n">
-        <v>-1.330385192772015e-07</v>
+        <v>-3.522706469824132e-07</v>
       </c>
       <c r="G74" t="n">
-        <v>6.835346350040714e-08</v>
+        <v>2.261243804549073e-07</v>
       </c>
     </row>
     <row r="75">
@@ -2161,10 +2161,10 @@
         <v>50</v>
       </c>
       <c r="F75" t="n">
-        <v>-1.078232755419792e-07</v>
+        <v>-4.02308778343626e-07</v>
       </c>
       <c r="G75" t="n">
-        <v>1.567067338882513e-08</v>
+        <v>3.258527931713226e-07</v>
       </c>
     </row>
     <row r="76">
@@ -2184,10 +2184,10 @@
         <v>60</v>
       </c>
       <c r="F76" t="n">
-        <v>-1.104384225288613e-07</v>
+        <v>-2.402125516378883e-07</v>
       </c>
       <c r="G76" t="n">
-        <v>3.372923979641938e-08</v>
+        <v>9.982444954585636e-08</v>
       </c>
     </row>
     <row r="77">
@@ -2207,10 +2207,10 @@
         <v>40</v>
       </c>
       <c r="F77" t="n">
-        <v>-2.119938004367042e-07</v>
+        <v>-3.153919378085527e-07</v>
       </c>
       <c r="G77" t="n">
-        <v>1.008139720938693e-07</v>
+        <v>1.866331902967127e-07</v>
       </c>
     </row>
     <row r="78">
@@ -2230,10 +2230,10 @@
         <v>50</v>
       </c>
       <c r="F78" t="n">
-        <v>-1.01070737557195e-07</v>
+        <v>-4.080333202764923e-07</v>
       </c>
       <c r="G78" t="n">
-        <v>5.317017311195413e-08</v>
+        <v>4.194459758299962e-07</v>
       </c>
     </row>
     <row r="79">
@@ -2253,10 +2253,10 @@
         <v>60</v>
       </c>
       <c r="F79" t="n">
-        <v>-9.83561363425361e-07</v>
+        <v>-3.588060756241048e-07</v>
       </c>
       <c r="G79" t="n">
-        <v>3.061866790512331e-07</v>
+        <v>2.765804435143245e-07</v>
       </c>
     </row>
     <row r="80">
@@ -2276,10 +2276,10 @@
         <v>40</v>
       </c>
       <c r="F80" t="n">
-        <v>-2.276344910466933e-07</v>
+        <v>-2.346146250586113e-07</v>
       </c>
       <c r="G80" t="n">
-        <v>1.400563553523221e-07</v>
+        <v>1.097275301844481e-07</v>
       </c>
     </row>
     <row r="81">
@@ -2299,10 +2299,10 @@
         <v>50</v>
       </c>
       <c r="F81" t="n">
-        <v>-5.384362643115217e-07</v>
+        <v>-2.026088046408377e-07</v>
       </c>
       <c r="G81" t="n">
-        <v>5.522050824700512e-07</v>
+        <v>5.405951150771954e-08</v>
       </c>
     </row>
     <row r="82">
@@ -2322,10 +2322,10 @@
         <v>60</v>
       </c>
       <c r="F82" t="n">
-        <v>-3.649607338733076e-07</v>
+        <v>-2.642886037051504e-07</v>
       </c>
       <c r="G82" t="n">
-        <v>4.213733840152792e-07</v>
+        <v>1.575801045183919e-07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>